<commit_message>
Added sections & flags. Omitted type conversions in .tt file.
</commit_message>
<xml_diff>
--- a/Example.xlsx
+++ b/Example.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Avi\Documents\Visual Studio 2022\Excel_CS\Excel_CS_sandbox\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA6159F7-663E-413B-8E3D-52FDA4E713B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{041DBA12-895A-4F84-8FC3-87351B841012}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{5E4BE526-7036-426A-B5CD-1241605C3F87}"/>
+    <workbookView xWindow="1950" yWindow="1950" windowWidth="21600" windowHeight="11835" xr2:uid="{5E4BE526-7036-426A-B5CD-1241605C3F87}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,18 +35,84 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="26">
+  <si>
+    <t>register</t>
+  </si>
+  <si>
+    <t>data</t>
+  </si>
+  <si>
+    <t>R[1:Reg_Test]</t>
+  </si>
+  <si>
+    <t>R[2:Reg_Test]</t>
+  </si>
+  <si>
+    <t>R[3:Reg_Test]</t>
+  </si>
+  <si>
+    <t>R[4:Reg_Test]</t>
+  </si>
+  <si>
+    <t>R[5:Reg_Test]</t>
+  </si>
+  <si>
+    <t>R[6:Reg_Test]</t>
+  </si>
+  <si>
+    <t>R[7:Reg_Test]</t>
+  </si>
+  <si>
+    <t>R[8:Reg_Test]</t>
+  </si>
+  <si>
+    <t>R[9:Reg_Test]</t>
+  </si>
+  <si>
+    <t>R[10:Reg_Test]</t>
+  </si>
+  <si>
+    <t>R[11:Reg_Test]</t>
+  </si>
+  <si>
+    <t>R[12:Reg_Test]</t>
+  </si>
+  <si>
+    <t>R[13:Reg_Test]</t>
+  </si>
+  <si>
+    <t>R[14:Reg_Test]</t>
+  </si>
+  <si>
+    <t>R[15:Reg_Test]</t>
+  </si>
+  <si>
+    <t>R[16:Reg_Test]</t>
+  </si>
+  <si>
+    <t>ON</t>
+  </si>
+  <si>
+    <t>OFF</t>
+  </si>
+  <si>
+    <t>F[20:Flg_Test]</t>
+  </si>
+  <si>
+    <t>F[21:Flg_Test]</t>
+  </si>
+  <si>
+    <t>F[22:Flg_Test]</t>
+  </si>
+  <si>
+    <t>F[23:FLg_Test]</t>
+  </si>
   <si>
     <t>isFlag</t>
   </si>
   <si>
-    <t>register</t>
-  </si>
-  <si>
-    <t>data</t>
-  </si>
-  <si>
-    <t>group</t>
+    <t>section</t>
   </si>
 </sst>
 </file>
@@ -400,31 +466,35 @@
   <dimension ref="A1:D21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="16.25" customWidth="1"/>
+    <col min="2" max="3" width="9.75" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>0</v>
+        <v>24</v>
       </c>
       <c r="D1" t="s">
-        <v>3</v>
+        <v>25</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2">
-        <v>30.5</v>
+      <c r="A2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B2" t="s">
+        <v>18</v>
       </c>
       <c r="C2" t="b">
         <f>TRUE</f>
@@ -435,11 +505,11 @@
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3">
-        <v>30.5</v>
+      <c r="A3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B3" t="s">
+        <v>19</v>
       </c>
       <c r="C3" t="b">
         <f>TRUE</f>
@@ -450,11 +520,11 @@
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4">
-        <v>3</v>
-      </c>
-      <c r="B4">
-        <v>30.5</v>
+      <c r="A4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B4" t="s">
+        <v>19</v>
       </c>
       <c r="C4" t="b">
         <f>TRUE</f>
@@ -465,11 +535,11 @@
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5">
-        <v>4</v>
-      </c>
-      <c r="B5">
-        <v>30.5</v>
+      <c r="A5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B5" t="s">
+        <v>18</v>
       </c>
       <c r="C5" t="b">
         <f>TRUE</f>
@@ -480,8 +550,8 @@
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A6">
-        <v>5</v>
+      <c r="A6" t="s">
+        <v>2</v>
       </c>
       <c r="B6">
         <v>30.5</v>
@@ -495,11 +565,11 @@
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A7">
-        <v>6</v>
+      <c r="A7" t="s">
+        <v>3</v>
       </c>
       <c r="B7">
-        <v>30.6</v>
+        <v>300</v>
       </c>
       <c r="C7" t="b">
         <f>FALSE</f>
@@ -510,8 +580,8 @@
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A8">
-        <v>7</v>
+      <c r="A8" t="s">
+        <v>4</v>
       </c>
       <c r="B8">
         <v>30.7</v>
@@ -525,8 +595,8 @@
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A9">
-        <v>8</v>
+      <c r="A9" t="s">
+        <v>5</v>
       </c>
       <c r="B9">
         <v>30.8</v>
@@ -540,8 +610,8 @@
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A10">
-        <v>9</v>
+      <c r="A10" t="s">
+        <v>6</v>
       </c>
       <c r="B10">
         <v>30.9</v>
@@ -555,8 +625,8 @@
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A11">
-        <v>10</v>
+      <c r="A11" t="s">
+        <v>7</v>
       </c>
       <c r="B11">
         <v>31</v>
@@ -570,8 +640,8 @@
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A12">
-        <v>11</v>
+      <c r="A12" t="s">
+        <v>8</v>
       </c>
       <c r="B12">
         <v>31.1</v>
@@ -585,8 +655,8 @@
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A13">
-        <v>12</v>
+      <c r="A13" t="s">
+        <v>9</v>
       </c>
       <c r="B13">
         <v>31.2</v>
@@ -600,8 +670,8 @@
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A14">
-        <v>13</v>
+      <c r="A14" t="s">
+        <v>10</v>
       </c>
       <c r="B14">
         <v>31.3</v>
@@ -615,8 +685,8 @@
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A15">
-        <v>14</v>
+      <c r="A15" t="s">
+        <v>11</v>
       </c>
       <c r="B15">
         <v>31.4</v>
@@ -630,8 +700,8 @@
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A16">
-        <v>15</v>
+      <c r="A16" t="s">
+        <v>12</v>
       </c>
       <c r="B16">
         <v>31.5</v>
@@ -645,8 +715,8 @@
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A17">
-        <v>16</v>
+      <c r="A17" t="s">
+        <v>13</v>
       </c>
       <c r="B17">
         <v>31.6</v>
@@ -660,8 +730,8 @@
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A18">
-        <v>17</v>
+      <c r="A18" t="s">
+        <v>14</v>
       </c>
       <c r="B18">
         <v>31.7</v>
@@ -675,8 +745,8 @@
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A19">
-        <v>18</v>
+      <c r="A19" t="s">
+        <v>15</v>
       </c>
       <c r="B19">
         <v>31.8</v>
@@ -690,8 +760,8 @@
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A20">
-        <v>19</v>
+      <c r="A20" t="s">
+        <v>16</v>
       </c>
       <c r="B20">
         <v>31.9</v>
@@ -705,8 +775,8 @@
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A21">
-        <v>20</v>
+      <c r="A21" t="s">
+        <v>17</v>
       </c>
       <c r="B21">
         <v>32</v>

</xml_diff>